<commit_message>
Finished automisation of import script with added batch identification. Transferred flying data in respective batch folder. Continued alignment automisation and updated qPCR run list.
</commit_message>
<xml_diff>
--- a/data/raw/Plasticity/qPCR_Run_list.xlsx
+++ b/data/raw/Plasticity/qPCR_Run_list.xlsx
@@ -33,6 +33,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">After speaking with Markus – better to run all reference genes with one sample group first to determine the optimal genes that lack differences in ct across tasks and subspecies</t>
         </r>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="32">
   <si>
     <t xml:space="preserve">Task</t>
   </si>
@@ -117,6 +118,9 @@
     <t xml:space="preserve">30/08/2022</t>
   </si>
   <si>
+    <t xml:space="preserve">31/08/2022</t>
+  </si>
+  <si>
     <t xml:space="preserve">Des2</t>
   </si>
   <si>
@@ -145,7 +149,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -179,11 +183,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -930,7 +929,7 @@
   <dimension ref="A1:D1019"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1002,8 +1001,11 @@
       <c r="A5" s="19" t="n">
         <v>4</v>
       </c>
+      <c r="B5" s="19" t="s">
+        <v>24</v>
+      </c>
       <c r="C5" s="20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5" s="19" t="n">
         <v>1</v>
@@ -1014,7 +1016,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D6" s="19" t="n">
         <v>2</v>
@@ -1025,7 +1027,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D7" s="19" t="n">
         <v>1</v>
@@ -1036,7 +1038,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D8" s="19" t="n">
         <v>2</v>
@@ -1047,7 +1049,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D9" s="19" t="n">
         <v>1</v>
@@ -1058,7 +1060,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D10" s="19" t="n">
         <v>2</v>
@@ -1069,7 +1071,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D11" s="19" t="n">
         <v>1</v>
@@ -1080,7 +1082,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D12" s="19" t="n">
         <v>1</v>
@@ -1091,7 +1093,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D13" s="19" t="n">
         <v>1</v>
@@ -1102,7 +1104,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D14" s="19" t="n">
         <v>1</v>
@@ -1124,7 +1126,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D16" s="19" t="n">
         <v>2</v>
@@ -1135,7 +1137,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D17" s="19" t="n">
         <v>2</v>
@@ -1146,7 +1148,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D18" s="19" t="n">
         <v>2</v>
@@ -1157,7 +1159,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D19" s="19" t="n">
         <v>2</v>

</xml_diff>

<commit_message>
Updated qPCR run list and continued work on automising alignment of chromatograms.
</commit_message>
<xml_diff>
--- a/data/raw/Plasticity/qPCR_Run_list.xlsx
+++ b/data/raw/Plasticity/qPCR_Run_list.xlsx
@@ -146,8 +146,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -272,7 +273,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -357,6 +358,14 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,7 +446,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -929,7 +938,7 @@
   <dimension ref="A1:D1019"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1015,6 +1024,9 @@
       <c r="A6" s="19" t="n">
         <v>5</v>
       </c>
+      <c r="B6" s="21" t="n">
+        <v>44805</v>
+      </c>
       <c r="C6" s="20" t="s">
         <v>25</v>
       </c>
@@ -1026,6 +1038,9 @@
       <c r="A7" s="19" t="n">
         <v>6</v>
       </c>
+      <c r="B7" s="21" t="n">
+        <v>44805</v>
+      </c>
       <c r="C7" s="20" t="s">
         <v>26</v>
       </c>
@@ -1037,6 +1052,7 @@
       <c r="A8" s="19" t="n">
         <v>7</v>
       </c>
+      <c r="B8" s="22"/>
       <c r="C8" s="20" t="s">
         <v>26</v>
       </c>
@@ -1048,6 +1064,7 @@
       <c r="A9" s="19" t="n">
         <v>8</v>
       </c>
+      <c r="B9" s="22"/>
       <c r="C9" s="20" t="s">
         <v>27</v>
       </c>
@@ -1059,6 +1076,7 @@
       <c r="A10" s="19" t="n">
         <v>9</v>
       </c>
+      <c r="B10" s="22"/>
       <c r="C10" s="20" t="s">
         <v>27</v>
       </c>
@@ -1070,6 +1088,7 @@
       <c r="A11" s="19" t="n">
         <v>10</v>
       </c>
+      <c r="B11" s="22"/>
       <c r="C11" s="20" t="s">
         <v>28</v>
       </c>
@@ -1081,6 +1100,7 @@
       <c r="A12" s="19" t="n">
         <v>11</v>
       </c>
+      <c r="B12" s="22"/>
       <c r="C12" s="20" t="s">
         <v>29</v>
       </c>
@@ -1092,6 +1112,7 @@
       <c r="A13" s="19" t="n">
         <v>12</v>
       </c>
+      <c r="B13" s="22"/>
       <c r="C13" s="20" t="s">
         <v>30</v>
       </c>
@@ -1103,6 +1124,7 @@
       <c r="A14" s="19" t="n">
         <v>13</v>
       </c>
+      <c r="B14" s="22"/>
       <c r="C14" s="20" t="s">
         <v>31</v>
       </c>
@@ -1114,6 +1136,7 @@
       <c r="A15" s="19" t="n">
         <v>14</v>
       </c>
+      <c r="B15" s="22"/>
       <c r="C15" s="20" t="s">
         <v>20</v>
       </c>
@@ -1125,6 +1148,7 @@
       <c r="A16" s="19" t="n">
         <v>15</v>
       </c>
+      <c r="B16" s="22"/>
       <c r="C16" s="20" t="s">
         <v>28</v>
       </c>
@@ -1136,6 +1160,7 @@
       <c r="A17" s="19" t="n">
         <v>16</v>
       </c>
+      <c r="B17" s="22"/>
       <c r="C17" s="20" t="s">
         <v>29</v>
       </c>
@@ -1147,6 +1172,7 @@
       <c r="A18" s="19" t="n">
         <v>17</v>
       </c>
+      <c r="B18" s="22"/>
       <c r="C18" s="20" t="s">
         <v>30</v>
       </c>
@@ -1158,6 +1184,7 @@
       <c r="A19" s="19" t="n">
         <v>18</v>
       </c>
+      <c r="B19" s="22"/>
       <c r="C19" s="20" t="s">
         <v>31</v>
       </c>

</xml_diff>